<commit_message>
OMU-2199 Add Sub User and field validations
OMU-2199 Add Sub User and field validations
> Added webdriver.manager.chromdriver and firefox driver, iedriver
> Added changes to base class
> Added Sub user account creation with read and write
> Added sub user with read only
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2EF05ACD-A67C-471B-B8E2-2903BFB1F628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New_Nordosn_Work\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C501A3-C444-47C6-BB61-C04C3533691F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17328" windowHeight="13224" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="AdminLogin" sheetId="1" r:id="rId2"/>
+    <sheet name="UserData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1:P24"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Password</t>
   </si>
@@ -37,6 +42,9 @@
   </si>
   <si>
     <t>raviuser@yopmail.com</t>
+  </si>
+  <si>
+    <t>autouser3@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -457,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450C58C-0634-4148-B924-699D95376F3E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,4 +535,42 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86030FE-F38A-4D5B-A289-B31333643154}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.77734375" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{286A2641-4B9E-48E5-9BEC-91D2B9AAF28B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LoginData excel file commit
LoginData excel file commit
exten-config.xml
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New_Nordosn_Work\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C501A3-C444-47C6-BB61-C04C3533691F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379FCAE8-59EE-4B37-8A20-76A25E09EDF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>raviuser@yopmail.com</t>
   </si>
   <si>
-    <t>autouser3@yopmail.com</t>
+    <t>autouser4@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
NOR XML Pressure changes
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -1,33 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2EF05ACD-A67C-471B-B8E2-2903BFB1F628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17328" windowHeight="13224" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="AdminLogin" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1:P24"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
+    <t>UserName</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>UserName</t>
+    <t>raviuser@yopmail.com</t>
   </si>
   <si>
     <t>amrendrasadmin@yopmail.com</t>
@@ -35,55 +31,198 @@
   <si>
     <t>pass1234</t>
   </si>
-  <si>
-    <t>raviuser@yopmail.com</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
+      <color indexed="30"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="30"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +241,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -126,33 +451,315 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="49" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{19DFC39A-23B0-4ADC-AB54-D047D0C5623A}"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Excel Built-in Normal" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -201,7 +808,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -234,26 +841,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -286,23 +876,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,87 +1017,85 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450C58C-0634-4148-B924-699D95376F3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="17.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>12345678</v>
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{71FEE756-8C55-41BC-B865-A20D4B8D72C6}"/>
+    <hyperlink ref="A2" r:id="rId1" display="raviuser@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E1DBC9-FCF4-45E5-B4FD-5A6169F6B019}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="18.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{841DF307-D1EC-4E8F-8D5B-CB32DF7D5C8F}"/>
+    <hyperlink ref="A2" r:id="rId1" display="amrendrasadmin@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
POC Create Issue in JIRA Client
POC Create Issue in JIRA Client
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New_Nordosn_Work\nordsonomu_automation\nordson.omu\src\test\java\com\nordson\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379FCAE8-59EE-4B37-8A20-76A25E09EDF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC09744-CF51-4C02-80FF-004DEA783277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DCA89EA-4F37-48B5-B8D2-472A325DFB74}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -41,10 +41,10 @@
     <t>pass1234</t>
   </si>
   <si>
-    <t>raviuser@yopmail.com</t>
+    <t>autouser4@yopmail.com</t>
   </si>
   <si>
-    <t>autouser4@yopmail.com</t>
+    <t>raviuser@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450C58C-0634-4148-B924-699D95376F3E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,10 +485,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>12345678</v>
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86030FE-F38A-4D5B-A289-B31333643154}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -561,7 +561,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>12345678</v>

</xml_diff>

<commit_message>
Default Pressure NOR file changes
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/LoginData.xlsx
@@ -37,12 +37,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +82,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -100,6 +93,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -110,7 +118,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,8 +161,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,39 +193,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,44 +210,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,187 +236,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,6 +441,36 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -476,17 +499,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,30 +515,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,157 +536,155 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1026,7 +1019,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1053,7 +1046,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="raviuser@yopmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="raviuser@yopmail.com" tooltip="mailto:raviuser@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>